<commit_message>
Initial framework for adding future resources
</commit_message>
<xml_diff>
--- a/analysis/library/pipeline/wc-pipeline.xlsx
+++ b/analysis/library/pipeline/wc-pipeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\West Coast ports\Analysis\Deployment\CORAL\analysis\library\pipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A3AEF4-2F73-4753-9385-48E7214DA149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349F0D7C-6714-4B82-94E6-43917873B9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{43706732-BCAE-BD4D-8F24-E09A39FF26FB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{43706732-BCAE-BD4D-8F24-E09A39FF26FB}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="4" r:id="rId1"/>
@@ -900,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0FC6D8E-5DF7-47FC-80AC-96398A94DDF7}">
   <dimension ref="A1:P56"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1012,7 +1012,7 @@
         <v>05/01/2029</v>
       </c>
       <c r="N2" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="O2" t="s">
         <v>117</v>
@@ -1062,7 +1062,7 @@
         <v>05/01/2030</v>
       </c>
       <c r="N3" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="O3" t="s">
         <v>117</v>
@@ -1112,7 +1112,7 @@
         <v>05/01/2031</v>
       </c>
       <c r="N4" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="O4" t="s">
         <v>117</v>
@@ -1169,8 +1169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D73D6878-E948-ED4B-8861-6367E17DF64F}">
   <dimension ref="A1:P56"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView zoomScale="54" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3039,8 +3039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5582B41F-4E13-B74C-AA14-3A857F30D199}">
   <dimension ref="A1:P56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="54" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView zoomScale="54" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -6386,21 +6386,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F8B0B258EEF50240929BB9F36779FA67" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="12d51bf3efa933eaa519000c321f81ab">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e15d5529-bdaf-4d9d-a53f-a8864ec66478" xmlns:ns3="d3fc4b62-afde-4d0a-b311-d84c0759faf2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="20035b3b5f1dea572bd5bfdac2fbef1b" ns2:_="" ns3:_="">
     <xsd:import namespace="e15d5529-bdaf-4d9d-a53f-a8864ec66478"/>
@@ -6565,24 +6550,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A122C20D-CA65-438C-8987-CA60D6F5CFCB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F67551D-9961-4E6F-8787-417C33DFD7BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E3D272-C267-4A9B-B8D3-2A1FB2B40D1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6599,4 +6582,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F67551D-9961-4E6F-8787-417C33DFD7BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A122C20D-CA65-438C-8987-CA60D6F5CFCB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Rename Port of San Luis consistently in input CSV, helpers.py
</commit_message>
<xml_diff>
--- a/analysis/library/pipeline/wc-pipeline.xlsx
+++ b/analysis/library/pipeline/wc-pipeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhemez/Floating-CORAL/CORAL/analysis/library/pipeline/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\West Coast ports\Analysis\Deployment\CORAL\analysis\library\pipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3FC0A8-CD8F-4B41-BC1D-54674EC18AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE76BA2E-A973-4CAF-815F-F0265B5F1760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34960" yWindow="2440" windowWidth="30320" windowHeight="17500" activeTab="1" xr2:uid="{43706732-BCAE-BD4D-8F24-E09A39FF26FB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{43706732-BCAE-BD4D-8F24-E09A39FF26FB}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="4" r:id="rId1"/>
@@ -707,7 +707,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Baseline-limited-ports"/>
@@ -1081,7 +1081,7 @@
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -1095,7 +1095,7 @@
     <col min="16" max="16" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1295,49 +1295,49 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="M16" s="20"/>
     </row>
-    <row r="43" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P43" s="12"/>
     </row>
-    <row r="44" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P44" s="12"/>
     </row>
-    <row r="45" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P45" s="12"/>
     </row>
-    <row r="46" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P46" s="12"/>
     </row>
-    <row r="47" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P47" s="12"/>
     </row>
-    <row r="48" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P48" s="12"/>
     </row>
-    <row r="49" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P49" s="12"/>
     </row>
-    <row r="50" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P50" s="12"/>
     </row>
-    <row r="51" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P51" s="12"/>
     </row>
-    <row r="52" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P52" s="12"/>
     </row>
-    <row r="53" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P53" s="12"/>
     </row>
-    <row r="54" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P54" s="12"/>
     </row>
-    <row r="55" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P55" s="12"/>
     </row>
-    <row r="56" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P56" s="12"/>
     </row>
   </sheetData>
@@ -1349,11 +1349,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D7E48D-8611-1746-819F-E119B83A8576}">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="F7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -1368,7 +1368,7 @@
     <col min="17" max="17" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -1421,7 +1421,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>53</v>
       </c>
@@ -3329,46 +3329,46 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="Q43" s="12"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="Q44" s="12"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="Q45" s="12"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="Q46" s="12"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="Q47" s="12"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="Q48" s="12"/>
     </row>
-    <row r="49" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q49" s="12"/>
     </row>
-    <row r="50" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="50" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q50" s="12"/>
     </row>
-    <row r="51" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q51" s="12"/>
     </row>
-    <row r="52" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="52" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q52" s="12"/>
     </row>
-    <row r="53" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="53" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q53" s="12"/>
     </row>
-    <row r="54" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q54" s="12"/>
     </row>
-    <row r="55" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q55" s="12"/>
     </row>
-    <row r="56" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="56" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q56" s="12"/>
     </row>
   </sheetData>
@@ -3384,7 +3384,7 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -3399,7 +3399,7 @@
     <col min="17" max="17" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -3722,7 +3722,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -3830,7 +3830,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -3884,7 +3884,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -3992,7 +3992,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -4100,7 +4100,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -4208,7 +4208,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -4262,7 +4262,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -4316,7 +4316,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -4532,7 +4532,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -4694,7 +4694,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -4748,7 +4748,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -4802,7 +4802,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -4856,7 +4856,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -4910,7 +4910,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -5018,7 +5018,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -5126,7 +5126,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -5180,7 +5180,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -5234,7 +5234,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -5288,7 +5288,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>53</v>
       </c>
@@ -5342,46 +5342,46 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="Q43" s="12"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="Q44" s="12"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="Q45" s="12"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="Q46" s="12"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="Q47" s="12"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="Q48" s="12"/>
     </row>
-    <row r="49" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q49" s="12"/>
     </row>
-    <row r="50" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="50" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q50" s="12"/>
     </row>
-    <row r="51" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q51" s="12"/>
     </row>
-    <row r="52" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="52" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q52" s="12"/>
     </row>
-    <row r="53" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="53" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q53" s="12"/>
     </row>
-    <row r="54" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q54" s="12"/>
     </row>
-    <row r="55" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q55" s="12"/>
     </row>
-    <row r="56" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="56" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q56" s="12"/>
     </row>
   </sheetData>
@@ -5393,11 +5393,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC05C72-3593-F349-9BDB-7CB43BC7148E}">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection sqref="A1:XFD46"/>
+    <sheetView topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31:N36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -5412,7 +5412,7 @@
     <col min="17" max="17" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -5465,7 +5465,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -5512,7 +5512,7 @@
         <v>05/01/2029</v>
       </c>
       <c r="N2" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="O2" t="s">
         <v>90</v>
@@ -5521,7 +5521,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -5568,7 +5568,7 @@
         <v>05/01/2030</v>
       </c>
       <c r="N3" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="O3" t="s">
         <v>90</v>
@@ -5577,7 +5577,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -5624,7 +5624,7 @@
         <v>05/01/2031</v>
       </c>
       <c r="N4" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="O4" t="s">
         <v>90</v>
@@ -5633,7 +5633,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -5687,7 +5687,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -5741,7 +5741,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -5849,7 +5849,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -5903,7 +5903,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -5957,7 +5957,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -6011,7 +6011,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -6065,7 +6065,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -6119,7 +6119,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -6173,7 +6173,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -6227,7 +6227,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -6281,7 +6281,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -6335,7 +6335,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -6389,7 +6389,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -6443,7 +6443,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -6551,7 +6551,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -6605,7 +6605,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -6659,7 +6659,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -6713,7 +6713,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -6767,7 +6767,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -6821,7 +6821,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -6875,7 +6875,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -6929,7 +6929,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -6983,7 +6983,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -7037,7 +7037,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -7084,7 +7084,7 @@
         <v>05/01/2032</v>
       </c>
       <c r="N31" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="O31" t="s">
         <v>90</v>
@@ -7093,7 +7093,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -7140,7 +7140,7 @@
         <v>05/01/2034</v>
       </c>
       <c r="N32" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="O32" t="s">
         <v>90</v>
@@ -7149,7 +7149,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -7196,7 +7196,7 @@
         <v>05/01/2036</v>
       </c>
       <c r="N33" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="O33" t="s">
         <v>90</v>
@@ -7205,7 +7205,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -7252,7 +7252,7 @@
         <v>05/01/2038</v>
       </c>
       <c r="N34" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="O34" t="s">
         <v>90</v>
@@ -7261,7 +7261,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -7308,7 +7308,7 @@
         <v>05/01/2040</v>
       </c>
       <c r="N35" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="O35" t="s">
         <v>90</v>
@@ -7317,7 +7317,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>53</v>
       </c>
@@ -7364,7 +7364,7 @@
         <v>05/01/2042</v>
       </c>
       <c r="N36" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="O36" t="s">
         <v>90</v>
@@ -7373,46 +7373,46 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="Q43" s="12"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="Q44" s="12"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="Q45" s="12"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="Q46" s="12"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="Q47" s="12"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="Q48" s="12"/>
     </row>
-    <row r="49" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q49" s="12"/>
     </row>
-    <row r="50" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="50" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q50" s="12"/>
     </row>
-    <row r="51" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q51" s="12"/>
     </row>
-    <row r="52" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="52" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q52" s="12"/>
     </row>
-    <row r="53" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="53" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q53" s="12"/>
     </row>
-    <row r="54" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q54" s="12"/>
     </row>
-    <row r="55" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q55" s="12"/>
     </row>
-    <row r="56" spans="17:17" x14ac:dyDescent="0.2">
+    <row r="56" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q56" s="12"/>
     </row>
   </sheetData>
@@ -7424,11 +7424,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E82BF5EA-4470-6E42-B4F0-EB0C845CDB6E}">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N49" sqref="N49:N56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -7443,7 +7443,7 @@
     <col min="17" max="17" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -7496,7 +7496,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -7550,7 +7550,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -7604,7 +7604,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -7658,7 +7658,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -7712,7 +7712,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -7766,7 +7766,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -7820,7 +7820,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -7874,7 +7874,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -7928,7 +7928,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -7982,7 +7982,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -8036,7 +8036,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -8090,7 +8090,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -8144,7 +8144,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -8198,7 +8198,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -8252,7 +8252,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -8306,7 +8306,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -8360,7 +8360,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -8414,7 +8414,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -8468,7 +8468,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -8522,7 +8522,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -8576,7 +8576,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -8630,7 +8630,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -8684,7 +8684,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -8738,7 +8738,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -8792,7 +8792,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -8846,7 +8846,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -8900,7 +8900,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -8954,7 +8954,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -9008,7 +9008,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -9062,7 +9062,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -9116,7 +9116,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -9170,7 +9170,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -9224,7 +9224,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -9278,7 +9278,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -9332,7 +9332,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>53</v>
       </c>
@@ -9386,7 +9386,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -9440,7 +9440,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>55</v>
       </c>
@@ -9494,7 +9494,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>56</v>
       </c>
@@ -9548,7 +9548,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>57</v>
       </c>
@@ -9602,7 +9602,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>58</v>
       </c>
@@ -9656,7 +9656,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>59</v>
       </c>
@@ -9710,7 +9710,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>60</v>
       </c>
@@ -9767,7 +9767,7 @@
       </c>
       <c r="Q43" s="12"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>61</v>
       </c>
@@ -9824,7 +9824,7 @@
       </c>
       <c r="Q44" s="12"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>62</v>
       </c>
@@ -9881,7 +9881,7 @@
       </c>
       <c r="Q45" s="12"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>63</v>
       </c>
@@ -9938,7 +9938,7 @@
       </c>
       <c r="Q46" s="12"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>64</v>
       </c>
@@ -9995,7 +9995,7 @@
       </c>
       <c r="Q47" s="12"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>65</v>
       </c>
@@ -10052,7 +10052,7 @@
       </c>
       <c r="Q48" s="12"/>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>66</v>
       </c>
@@ -10099,7 +10099,7 @@
         <v>05/01/2039</v>
       </c>
       <c r="N49" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="O49" t="s">
         <v>112</v>
@@ -10109,7 +10109,7 @@
       </c>
       <c r="Q49" s="12"/>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>67</v>
       </c>
@@ -10156,7 +10156,7 @@
         <v>05/01/2040</v>
       </c>
       <c r="N50" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="O50" t="s">
         <v>112</v>
@@ -10166,7 +10166,7 @@
       </c>
       <c r="Q50" s="12"/>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>68</v>
       </c>
@@ -10213,7 +10213,7 @@
         <v>05/01/2041</v>
       </c>
       <c r="N51" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="O51" t="s">
         <v>112</v>
@@ -10223,7 +10223,7 @@
       </c>
       <c r="Q51" s="12"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>69</v>
       </c>
@@ -10270,7 +10270,7 @@
         <v>05/01/2042</v>
       </c>
       <c r="N52" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="O52" t="s">
         <v>112</v>
@@ -10280,7 +10280,7 @@
       </c>
       <c r="Q52" s="12"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>70</v>
       </c>
@@ -10327,7 +10327,7 @@
         <v>05/01/2043</v>
       </c>
       <c r="N53" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="O53" t="s">
         <v>112</v>
@@ -10337,7 +10337,7 @@
       </c>
       <c r="Q53" s="12"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>71</v>
       </c>
@@ -10384,7 +10384,7 @@
         <v>05/01/2044</v>
       </c>
       <c r="N54" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="O54" t="s">
         <v>112</v>
@@ -10394,7 +10394,7 @@
       </c>
       <c r="Q54" s="12"/>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>72</v>
       </c>
@@ -10441,7 +10441,7 @@
         <v>05/01/2041</v>
       </c>
       <c r="N55" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="O55" t="s">
         <v>114</v>
@@ -10451,7 +10451,7 @@
       </c>
       <c r="Q55" s="12"/>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>73</v>
       </c>
@@ -10498,7 +10498,7 @@
         <v>05/01/2043</v>
       </c>
       <c r="N56" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="O56" t="s">
         <v>114</v>
@@ -10517,11 +10517,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{359DCE26-3DE6-DA4E-ADD0-DA93F4839E90}">
   <dimension ref="A2:O30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
@@ -10535,12 +10535,12 @@
     <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -10551,7 +10551,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -10559,7 +10559,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>81</v>
       </c>
@@ -10567,7 +10567,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>83</v>
       </c>
@@ -10575,7 +10575,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>100</v>
       </c>
@@ -10602,7 +10602,7 @@
       </c>
       <c r="O8" s="22"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="10"/>
       <c r="B9" s="6"/>
       <c r="C9" s="4" t="s">
@@ -10645,7 +10645,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="23" t="s">
         <v>101</v>
       </c>
@@ -10672,7 +10672,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="23"/>
       <c r="B11" s="5" t="s">
         <v>97</v>
@@ -10697,7 +10697,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="23"/>
       <c r="B12" s="5" t="s">
         <v>98</v>
@@ -10724,7 +10724,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="23"/>
       <c r="B13" s="5" t="s">
         <v>99</v>
@@ -10753,7 +10753,7 @@
       </c>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="23"/>
       <c r="B14" s="8" t="s">
         <v>14</v>
@@ -10776,10 +10776,10 @@
         <v>109.724</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="62" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
         <v>115</v>
       </c>
@@ -10799,7 +10799,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>120</v>
       </c>
@@ -10817,7 +10817,7 @@
       </c>
       <c r="F18" s="17"/>
     </row>
-    <row r="19" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A19" s="16" t="s">
         <v>125</v>
       </c>
@@ -10837,7 +10837,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A20" s="16" t="s">
         <v>131</v>
       </c>
@@ -10857,7 +10857,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
         <v>137</v>
       </c>
@@ -10871,7 +10871,7 @@
         <v>89.117000000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="s">
         <v>138</v>
       </c>
@@ -10891,12 +10891,12 @@
         <v>913</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
         <v>139</v>
       </c>
@@ -10919,7 +10919,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
         <v>140</v>
       </c>
@@ -10930,7 +10930,7 @@
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
         <v>141</v>
       </c>
@@ -10941,7 +10941,7 @@
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="13" t="s">
         <v>142</v>
       </c>
@@ -10952,7 +10952,7 @@
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
         <v>143</v>
       </c>
@@ -10976,12 +10976,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11150,15 +11147,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F67551D-9961-4E6F-8787-417C33DFD7BB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A122C20D-CA65-438C-8987-CA60D6F5CFCB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11183,10 +11184,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A122C20D-CA65-438C-8987-CA60D6F5CFCB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F67551D-9961-4E6F-8787-417C33DFD7BB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added initial port online scheduling
</commit_message>
<xml_diff>
--- a/analysis/library/pipeline/wc-pipeline.xlsx
+++ b/analysis/library/pipeline/wc-pipeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\West Coast ports\Analysis\Deployment\CORAL\analysis\library\pipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE76BA2E-A973-4CAF-815F-F0265B5F1760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505CDB3D-AF1D-4AB9-8D24-6138ABF3217B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{43706732-BCAE-BD4D-8F24-E09A39FF26FB}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="151">
   <si>
     <t>lat</t>
   </si>
@@ -490,6 +490,24 @@
   </si>
   <si>
     <t>Scenarios and corresponding S&amp;I ports</t>
+  </si>
+  <si>
+    <t>Port capacity scheduling</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>Available date for each production line (sub assembly + turbine integration)</t>
+  </si>
+  <si>
+    <t>Line #1</t>
+  </si>
+  <si>
+    <t>Line #2</t>
+  </si>
+  <si>
+    <t>Line #3</t>
   </si>
 </sst>
 </file>
@@ -5393,7 +5411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC05C72-3593-F349-9BDB-7CB43BC7148E}">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N31" sqref="N31:N36"/>
     </sheetView>
   </sheetViews>
@@ -7424,8 +7442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E82BF5EA-4470-6E42-B4F0-EB0C845CDB6E}">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N49" sqref="N49:N56"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -9757,7 +9775,7 @@
         <v>05/01/2038</v>
       </c>
       <c r="N43" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O43" t="s">
         <v>92</v>
@@ -9814,7 +9832,7 @@
         <v>05/01/2040</v>
       </c>
       <c r="N44" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O44" t="s">
         <v>91</v>
@@ -9871,7 +9889,7 @@
         <v>05/01/2041</v>
       </c>
       <c r="N45" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O45" t="s">
         <v>92</v>
@@ -9928,7 +9946,7 @@
         <v>05/01/2042</v>
       </c>
       <c r="N46" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O46" t="s">
         <v>91</v>
@@ -9985,7 +10003,7 @@
         <v>05/01/2043</v>
       </c>
       <c r="N47" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O47" t="s">
         <v>92</v>
@@ -10042,7 +10060,7 @@
         <v>05/01/2044</v>
       </c>
       <c r="N48" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O48" t="s">
         <v>91</v>
@@ -10515,10 +10533,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{359DCE26-3DE6-DA4E-ADD0-DA93F4839E90}">
-  <dimension ref="A2:O30"/>
+  <dimension ref="A2:O40"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -10963,6 +10981,79 @@
       <c r="F30" s="19"/>
       <c r="G30" s="19"/>
     </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>146</v>
+      </c>
+      <c r="B35" t="s">
+        <v>148</v>
+      </c>
+      <c r="C35" t="s">
+        <v>149</v>
+      </c>
+      <c r="D35" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36">
+        <v>2028</v>
+      </c>
+      <c r="C36">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37">
+        <v>2032</v>
+      </c>
+      <c r="C37">
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39">
+        <v>2031</v>
+      </c>
+      <c r="C39">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40">
+        <v>2039</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C8:E8"/>
@@ -10982,6 +11073,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F8B0B258EEF50240929BB9F36779FA67" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="12d51bf3efa933eaa519000c321f81ab">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e15d5529-bdaf-4d9d-a53f-a8864ec66478" xmlns:ns3="d3fc4b62-afde-4d0a-b311-d84c0759faf2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="20035b3b5f1dea572bd5bfdac2fbef1b" ns2:_="" ns3:_="">
     <xsd:import namespace="e15d5529-bdaf-4d9d-a53f-a8864ec66478"/>
@@ -11146,15 +11246,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A122C20D-CA65-438C-8987-CA60D6F5CFCB}">
   <ds:schemaRefs>
@@ -11165,6 +11256,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F67551D-9961-4E6F-8787-417C33DFD7BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E3D272-C267-4A9B-B8D3-2A1FB2B40D1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11181,12 +11280,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F67551D-9961-4E6F-8787-417C33DFD7BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Concat weather time series to last full simulation. Add phase dependencies to CORAL/pipelines.py
</commit_message>
<xml_diff>
--- a/analysis/library/pipeline/wc-pipeline.xlsx
+++ b/analysis/library/pipeline/wc-pipeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\West Coast ports\Analysis\Deployment\CORAL\analysis\library\pipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505CDB3D-AF1D-4AB9-8D24-6138ABF3217B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C783DE08-6E08-434E-8896-26EFCD6F1CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{43706732-BCAE-BD4D-8F24-E09A39FF26FB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{43706732-BCAE-BD4D-8F24-E09A39FF26FB}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="4" r:id="rId1"/>
@@ -1095,8 +1095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0FC6D8E-5DF7-47FC-80AC-96398A94DDF7}">
   <dimension ref="A1:P56"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1207,7 +1207,7 @@
         <v>05/01/2029</v>
       </c>
       <c r="N2" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="O2" t="s">
         <v>103</v>
@@ -1257,7 +1257,7 @@
         <v>05/01/2030</v>
       </c>
       <c r="N3" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="O3" t="s">
         <v>103</v>
@@ -1307,7 +1307,7 @@
         <v>05/01/2031</v>
       </c>
       <c r="N4" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="O4" t="s">
         <v>103</v>
@@ -7442,7 +7442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E82BF5EA-4470-6E42-B4F0-EB0C845CDB6E}">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
@@ -11067,18 +11067,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11247,18 +11247,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A122C20D-CA65-438C-8987-CA60D6F5CFCB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F67551D-9961-4E6F-8787-417C33DFD7BB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F67551D-9961-4E6F-8787-417C33DFD7BB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A122C20D-CA65-438C-8987-CA60D6F5CFCB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Run with expanded port production lines
</commit_message>
<xml_diff>
--- a/analysis/library/pipeline/wc-pipeline.xlsx
+++ b/analysis/library/pipeline/wc-pipeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\West Coast ports\Analysis\Deployment\CORAL\analysis\library\pipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C783DE08-6E08-434E-8896-26EFCD6F1CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E677AC-BA77-4682-96B7-B1AAB371566D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{43706732-BCAE-BD4D-8F24-E09A39FF26FB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="5" xr2:uid="{43706732-BCAE-BD4D-8F24-E09A39FF26FB}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="4" r:id="rId1"/>
@@ -1095,7 +1095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0FC6D8E-5DF7-47FC-80AC-96398A94DDF7}">
   <dimension ref="A1:P56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
@@ -10535,8 +10535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{359DCE26-3DE6-DA4E-ADD0-DA93F4839E90}">
   <dimension ref="A2:O40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="70" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -11067,21 +11067,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F8B0B258EEF50240929BB9F36779FA67" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="12d51bf3efa933eaa519000c321f81ab">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e15d5529-bdaf-4d9d-a53f-a8864ec66478" xmlns:ns3="d3fc4b62-afde-4d0a-b311-d84c0759faf2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="20035b3b5f1dea572bd5bfdac2fbef1b" ns2:_="" ns3:_="">
     <xsd:import namespace="e15d5529-bdaf-4d9d-a53f-a8864ec66478"/>
@@ -11246,24 +11231,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F67551D-9961-4E6F-8787-417C33DFD7BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A122C20D-CA65-438C-8987-CA60D6F5CFCB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E3D272-C267-4A9B-B8D3-2A1FB2B40D1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11280,4 +11263,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A122C20D-CA65-438C-8987-CA60D6F5CFCB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F67551D-9961-4E6F-8787-417C33DFD7BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Iterate on expanded scenarios and tow vessels
</commit_message>
<xml_diff>
--- a/analysis/library/pipeline/wc-pipeline.xlsx
+++ b/analysis/library/pipeline/wc-pipeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhemez/Floating-CORAL/CORAL/analysis/library/pipeline/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\West Coast ports\Analysis\Deployment\CORAL\analysis\library\pipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD62379-84BE-9C4B-A064-1DE622E07062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855A8DA3-5BA6-431B-AD2F-9BA0D523947C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="960" windowWidth="26380" windowHeight="16100" activeTab="4" xr2:uid="{43706732-BCAE-BD4D-8F24-E09A39FF26FB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="6" xr2:uid="{43706732-BCAE-BD4D-8F24-E09A39FF26FB}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="4" r:id="rId1"/>
@@ -786,7 +786,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Baseline-limited-ports"/>
@@ -1160,7 +1160,7 @@
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -1174,7 +1174,7 @@
     <col min="16" max="16" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1374,49 +1374,49 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="M16" s="20"/>
     </row>
-    <row r="43" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P43" s="12"/>
     </row>
-    <row r="44" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P44" s="12"/>
     </row>
-    <row r="45" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P45" s="12"/>
     </row>
-    <row r="46" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P46" s="12"/>
     </row>
-    <row r="47" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P47" s="12"/>
     </row>
-    <row r="48" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P48" s="12"/>
     </row>
-    <row r="49" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P49" s="12"/>
     </row>
-    <row r="50" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P50" s="12"/>
     </row>
-    <row r="51" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P51" s="12"/>
     </row>
-    <row r="52" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P52" s="12"/>
     </row>
-    <row r="53" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P53" s="12"/>
     </row>
-    <row r="54" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P54" s="12"/>
     </row>
-    <row r="55" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P55" s="12"/>
     </row>
-    <row r="56" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P56" s="12"/>
     </row>
   </sheetData>
@@ -1432,7 +1432,7 @@
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -1448,7 +1448,7 @@
     <col min="18" max="18" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -2929,46 +2929,46 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R33" s="12"/>
     </row>
-    <row r="34" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R34" s="12"/>
     </row>
-    <row r="35" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R35" s="12"/>
     </row>
-    <row r="36" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R36" s="12"/>
     </row>
-    <row r="37" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R37" s="12"/>
     </row>
-    <row r="38" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R38" s="12"/>
     </row>
-    <row r="39" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R39" s="12"/>
     </row>
-    <row r="40" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R40" s="12"/>
     </row>
-    <row r="41" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R41" s="12"/>
     </row>
-    <row r="42" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R42" s="12"/>
     </row>
-    <row r="43" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R43" s="12"/>
     </row>
-    <row r="44" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R44" s="12"/>
     </row>
-    <row r="45" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R45" s="12"/>
     </row>
-    <row r="46" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R46" s="12"/>
     </row>
   </sheetData>
@@ -2984,7 +2984,7 @@
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -3000,7 +3000,7 @@
     <col min="18" max="18" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -3686,7 +3686,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -3857,7 +3857,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -4142,7 +4142,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -4258,7 +4258,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -4316,7 +4316,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -4374,7 +4374,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -4432,7 +4432,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -4490,46 +4490,46 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R33" s="12"/>
     </row>
-    <row r="34" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R34" s="12"/>
     </row>
-    <row r="35" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R35" s="12"/>
     </row>
-    <row r="36" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R36" s="12"/>
     </row>
-    <row r="37" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R37" s="12"/>
     </row>
-    <row r="38" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R38" s="12"/>
     </row>
-    <row r="39" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R39" s="12"/>
     </row>
-    <row r="40" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R40" s="12"/>
     </row>
-    <row r="41" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R41" s="12"/>
     </row>
-    <row r="42" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R42" s="12"/>
     </row>
-    <row r="43" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R43" s="12"/>
     </row>
-    <row r="44" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R44" s="12"/>
     </row>
-    <row r="45" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R45" s="12"/>
     </row>
-    <row r="46" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R46" s="12"/>
     </row>
   </sheetData>
@@ -4545,7 +4545,7 @@
       <selection activeCell="P36" sqref="P36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -4561,7 +4561,7 @@
     <col min="18" max="18" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -4617,7 +4617,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -4676,7 +4676,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -4851,7 +4851,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -4908,7 +4908,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -4965,7 +4965,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -5022,7 +5022,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -5136,7 +5136,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -5250,7 +5250,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -5307,7 +5307,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -5364,7 +5364,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -5421,7 +5421,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -5535,7 +5535,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -5592,7 +5592,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -5649,7 +5649,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -5706,7 +5706,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -5824,7 +5824,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -5883,7 +5883,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -5942,7 +5942,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -6001,7 +6001,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -6060,46 +6060,46 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R33" s="12"/>
     </row>
-    <row r="34" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R34" s="12"/>
     </row>
-    <row r="35" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R35" s="12"/>
     </row>
-    <row r="36" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R36" s="12"/>
     </row>
-    <row r="37" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R37" s="12"/>
     </row>
-    <row r="38" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R38" s="12"/>
     </row>
-    <row r="39" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R39" s="12"/>
     </row>
-    <row r="40" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R40" s="12"/>
     </row>
-    <row r="41" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R41" s="12"/>
     </row>
-    <row r="42" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R42" s="12"/>
     </row>
-    <row r="43" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R43" s="12"/>
     </row>
-    <row r="44" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R44" s="12"/>
     </row>
-    <row r="45" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R45" s="12"/>
     </row>
-    <row r="46" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R46" s="12"/>
     </row>
   </sheetData>
@@ -6112,11 +6112,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D7E48D-8611-1746-819F-E119B83A8576}">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -6132,7 +6132,7 @@
     <col min="18" max="18" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -6188,7 +6188,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -6247,7 +6247,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -6365,7 +6365,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -6422,7 +6422,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -6479,7 +6479,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -6536,7 +6536,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -6593,7 +6593,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -6650,7 +6650,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -6707,7 +6707,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -6764,7 +6764,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -6821,7 +6821,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -6878,7 +6878,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -6935,7 +6935,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -6992,7 +6992,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -7049,7 +7049,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -7106,7 +7106,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -7163,7 +7163,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -7220,7 +7220,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -7277,7 +7277,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -7334,7 +7334,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -7391,7 +7391,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -7448,7 +7448,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -7505,7 +7505,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -7562,7 +7562,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -7619,7 +7619,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -7676,7 +7676,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -7733,7 +7733,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -7790,7 +7790,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -7847,7 +7847,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -7906,7 +7906,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -7965,7 +7965,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -8024,7 +8024,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -8083,7 +8083,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -8142,7 +8142,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>53</v>
       </c>
@@ -8201,77 +8201,77 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C37" s="22"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C38" s="22"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C39" s="22"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C40" s="22"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C41" s="22"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C42" s="22"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C43" s="22"/>
       <c r="R43" s="12"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C44" s="22"/>
       <c r="R44" s="12"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C45" s="22"/>
       <c r="R45" s="12"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C46" s="22"/>
       <c r="R46" s="12"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C47" s="22"/>
       <c r="R47" s="12"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C48" s="22"/>
       <c r="R48" s="12"/>
     </row>
-    <row r="49" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C49" s="22"/>
       <c r="R49" s="12"/>
     </row>
-    <row r="50" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C50" s="22"/>
       <c r="R50" s="12"/>
     </row>
-    <row r="51" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C51" s="22"/>
       <c r="R51" s="12"/>
     </row>
-    <row r="52" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C52" s="22"/>
       <c r="R52" s="12"/>
     </row>
-    <row r="53" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C53" s="22"/>
       <c r="R53" s="12"/>
     </row>
-    <row r="54" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C54" s="22"/>
       <c r="R54" s="12"/>
     </row>
-    <row r="55" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C55" s="22"/>
       <c r="R55" s="12"/>
     </row>
-    <row r="56" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C56" s="22"/>
       <c r="R56" s="12"/>
     </row>
@@ -8288,7 +8288,7 @@
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -8304,7 +8304,7 @@
     <col min="18" max="18" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -8360,7 +8360,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -8417,7 +8417,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -8474,7 +8474,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -8531,7 +8531,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -8588,7 +8588,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -8645,7 +8645,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -8702,7 +8702,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -8759,7 +8759,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -8816,7 +8816,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -8873,7 +8873,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -8930,7 +8930,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -8987,7 +8987,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -9044,7 +9044,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -9101,7 +9101,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -9158,7 +9158,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -9215,7 +9215,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -9272,7 +9272,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -9329,7 +9329,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -9386,7 +9386,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -9443,7 +9443,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -9500,7 +9500,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -9557,7 +9557,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -9614,7 +9614,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -9671,7 +9671,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -9728,7 +9728,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -9785,7 +9785,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -9842,7 +9842,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -9899,7 +9899,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -9956,7 +9956,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -10013,7 +10013,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -10070,7 +10070,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -10127,7 +10127,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -10184,7 +10184,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -10241,7 +10241,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -10298,7 +10298,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>53</v>
       </c>
@@ -10355,46 +10355,46 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="R43" s="12"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="R44" s="12"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="R45" s="12"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="R46" s="12"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="R47" s="12"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="R48" s="12"/>
     </row>
-    <row r="49" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="49" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R49" s="12"/>
     </row>
-    <row r="50" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="50" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R50" s="12"/>
     </row>
-    <row r="51" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="51" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R51" s="12"/>
     </row>
-    <row r="52" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="52" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R52" s="12"/>
     </row>
-    <row r="53" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="53" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R53" s="12"/>
     </row>
-    <row r="54" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="54" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R54" s="12"/>
     </row>
-    <row r="55" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="55" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R55" s="12"/>
     </row>
-    <row r="56" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="56" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R56" s="12"/>
     </row>
   </sheetData>
@@ -10406,11 +10406,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E82BF5EA-4470-6E42-B4F0-EB0C845CDB6E}">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="O50" sqref="O49:O50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -10426,7 +10426,7 @@
     <col min="18" max="18" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -10482,7 +10482,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -10539,7 +10539,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -10596,7 +10596,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -10653,7 +10653,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -10710,7 +10710,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -10767,7 +10767,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -10824,7 +10824,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -10881,7 +10881,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -10938,7 +10938,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -10995,7 +10995,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -11052,7 +11052,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -11109,7 +11109,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -11166,7 +11166,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -11223,7 +11223,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -11280,7 +11280,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -11337,7 +11337,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -11394,7 +11394,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -11451,7 +11451,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -11508,7 +11508,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -11565,7 +11565,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -11622,7 +11622,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -11679,7 +11679,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -11736,7 +11736,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -11793,7 +11793,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -11850,7 +11850,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -11907,7 +11907,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -11964,7 +11964,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -12021,7 +12021,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -12078,7 +12078,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -12135,7 +12135,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -12192,7 +12192,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -12249,7 +12249,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -12306,7 +12306,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -12354,7 +12354,7 @@
         <v>05/01/2038</v>
       </c>
       <c r="O34" t="s">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="P34" t="s">
         <v>90</v>
@@ -12363,7 +12363,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -12411,7 +12411,7 @@
         <v>05/01/2040</v>
       </c>
       <c r="O35" t="s">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="P35" t="s">
         <v>90</v>
@@ -12420,7 +12420,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>53</v>
       </c>
@@ -12468,7 +12468,7 @@
         <v>05/01/2042</v>
       </c>
       <c r="O36" t="s">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="P36" t="s">
         <v>90</v>
@@ -12477,7 +12477,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -12534,7 +12534,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>55</v>
       </c>
@@ -12591,7 +12591,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>56</v>
       </c>
@@ -12648,7 +12648,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>57</v>
       </c>
@@ -12705,7 +12705,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>58</v>
       </c>
@@ -12762,7 +12762,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>59</v>
       </c>
@@ -12819,7 +12819,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>60</v>
       </c>
@@ -12879,7 +12879,7 @@
       </c>
       <c r="R43" s="12"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>61</v>
       </c>
@@ -12929,7 +12929,7 @@
         <v>05/01/2040</v>
       </c>
       <c r="O44" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="P44" t="s">
         <v>91</v>
@@ -12939,7 +12939,7 @@
       </c>
       <c r="R44" s="12"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>62</v>
       </c>
@@ -12999,7 +12999,7 @@
       </c>
       <c r="R45" s="12"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>63</v>
       </c>
@@ -13049,7 +13049,7 @@
         <v>05/01/2042</v>
       </c>
       <c r="O46" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="P46" t="s">
         <v>91</v>
@@ -13059,7 +13059,7 @@
       </c>
       <c r="R46" s="12"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>64</v>
       </c>
@@ -13119,7 +13119,7 @@
       </c>
       <c r="R47" s="12"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>65</v>
       </c>
@@ -13169,7 +13169,7 @@
         <v>05/01/2044</v>
       </c>
       <c r="O48" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="P48" t="s">
         <v>91</v>
@@ -13179,7 +13179,7 @@
       </c>
       <c r="R48" s="12"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>66</v>
       </c>
@@ -13228,8 +13228,8 @@
         <f>_xlfn.CONCAT([1]Helpers!$B$4,'Expanded-High'!M49)</f>
         <v>05/01/2039</v>
       </c>
-      <c r="O49" s="25" t="s">
-        <v>75</v>
+      <c r="O49" t="s">
+        <v>10</v>
       </c>
       <c r="P49" t="s">
         <v>112</v>
@@ -13239,7 +13239,7 @@
       </c>
       <c r="R49" s="12"/>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>67</v>
       </c>
@@ -13288,8 +13288,8 @@
         <f>_xlfn.CONCAT([1]Helpers!$B$4,'Expanded-High'!M50)</f>
         <v>05/01/2040</v>
       </c>
-      <c r="O50" s="25" t="s">
-        <v>75</v>
+      <c r="O50" t="s">
+        <v>10</v>
       </c>
       <c r="P50" t="s">
         <v>112</v>
@@ -13299,7 +13299,7 @@
       </c>
       <c r="R50" s="12"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>68</v>
       </c>
@@ -13348,8 +13348,8 @@
         <f>_xlfn.CONCAT([1]Helpers!$B$4,'Expanded-High'!M51)</f>
         <v>05/01/2041</v>
       </c>
-      <c r="O51" s="25" t="s">
-        <v>75</v>
+      <c r="O51" t="s">
+        <v>10</v>
       </c>
       <c r="P51" t="s">
         <v>112</v>
@@ -13359,7 +13359,7 @@
       </c>
       <c r="R51" s="12"/>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>69</v>
       </c>
@@ -13408,8 +13408,8 @@
         <f>_xlfn.CONCAT([1]Helpers!$B$4,'Expanded-High'!M52)</f>
         <v>05/01/2042</v>
       </c>
-      <c r="O52" s="25" t="s">
-        <v>75</v>
+      <c r="O52" t="s">
+        <v>10</v>
       </c>
       <c r="P52" t="s">
         <v>112</v>
@@ -13419,7 +13419,7 @@
       </c>
       <c r="R52" s="12"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>70</v>
       </c>
@@ -13468,8 +13468,8 @@
         <f>_xlfn.CONCAT([1]Helpers!$B$4,'Expanded-High'!M53)</f>
         <v>05/01/2043</v>
       </c>
-      <c r="O53" s="25" t="s">
-        <v>75</v>
+      <c r="O53" t="s">
+        <v>10</v>
       </c>
       <c r="P53" t="s">
         <v>112</v>
@@ -13479,7 +13479,7 @@
       </c>
       <c r="R53" s="12"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>71</v>
       </c>
@@ -13528,8 +13528,8 @@
         <f>_xlfn.CONCAT([1]Helpers!$B$4,'Expanded-High'!M54)</f>
         <v>05/01/2044</v>
       </c>
-      <c r="O54" s="25" t="s">
-        <v>75</v>
+      <c r="O54" t="s">
+        <v>10</v>
       </c>
       <c r="P54" t="s">
         <v>112</v>
@@ -13539,7 +13539,7 @@
       </c>
       <c r="R54" s="12"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>72</v>
       </c>
@@ -13588,7 +13588,7 @@
         <f>_xlfn.CONCAT([1]Helpers!$B$4,'Expanded-High'!M55)</f>
         <v>05/01/2041</v>
       </c>
-      <c r="O55" s="25" t="s">
+      <c r="O55" t="s">
         <v>75</v>
       </c>
       <c r="P55" t="s">
@@ -13599,7 +13599,7 @@
       </c>
       <c r="R55" s="12"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>73</v>
       </c>
@@ -13648,7 +13648,7 @@
         <f>_xlfn.CONCAT([1]Helpers!$B$4,'Expanded-High'!M56)</f>
         <v>05/01/2043</v>
       </c>
-      <c r="O56" s="25" t="s">
+      <c r="O56" t="s">
         <v>75</v>
       </c>
       <c r="P56" t="s">
@@ -13672,7 +13672,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
@@ -13686,12 +13686,12 @@
     <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -13702,7 +13702,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -13710,7 +13710,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>81</v>
       </c>
@@ -13718,7 +13718,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>83</v>
       </c>
@@ -13726,7 +13726,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>100</v>
       </c>
@@ -13753,7 +13753,7 @@
       </c>
       <c r="O8" s="27"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="10"/>
       <c r="B9" s="6"/>
       <c r="C9" s="4" t="s">
@@ -13796,7 +13796,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="28" t="s">
         <v>101</v>
       </c>
@@ -13823,7 +13823,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="28"/>
       <c r="B11" s="5" t="s">
         <v>97</v>
@@ -13848,7 +13848,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="28"/>
       <c r="B12" s="5" t="s">
         <v>98</v>
@@ -13875,7 +13875,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="28"/>
       <c r="B13" s="5" t="s">
         <v>99</v>
@@ -13904,7 +13904,7 @@
       </c>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="28"/>
       <c r="B14" s="8" t="s">
         <v>14</v>
@@ -13927,10 +13927,10 @@
         <v>109.724</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="62" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
         <v>115</v>
       </c>
@@ -13950,7 +13950,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>120</v>
       </c>
@@ -13968,7 +13968,7 @@
       </c>
       <c r="F18" s="17"/>
     </row>
-    <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A19" s="16" t="s">
         <v>125</v>
       </c>
@@ -13988,7 +13988,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A20" s="16" t="s">
         <v>131</v>
       </c>
@@ -14008,7 +14008,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
         <v>137</v>
       </c>
@@ -14022,7 +14022,7 @@
         <v>89.117000000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="s">
         <v>138</v>
       </c>
@@ -14042,12 +14042,12 @@
         <v>913</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
         <v>139</v>
       </c>
@@ -14067,7 +14067,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
         <v>151</v>
       </c>
@@ -14077,7 +14077,7 @@
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
         <v>152</v>
       </c>
@@ -14087,7 +14087,7 @@
       <c r="E28" s="24"/>
       <c r="F28" s="13"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="13" t="s">
         <v>153</v>
       </c>
@@ -14097,7 +14097,7 @@
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
         <v>154</v>
       </c>
@@ -14107,7 +14107,7 @@
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
         <v>155</v>
       </c>
@@ -14117,7 +14117,7 @@
       <c r="E31" s="19"/>
       <c r="F31" s="13"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
         <v>156</v>
       </c>
@@ -14127,17 +14127,17 @@
       <c r="E32" s="23"/>
       <c r="F32" s="23"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>142</v>
       </c>
@@ -14151,7 +14151,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -14162,7 +14162,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -14173,7 +14173,7 @@
         <v>2034</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>75</v>
       </c>
@@ -14181,7 +14181,7 @@
         <v>2037</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -14192,7 +14192,7 @@
         <v>2038</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -14219,15 +14219,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F8B0B258EEF50240929BB9F36779FA67" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="12d51bf3efa933eaa519000c321f81ab">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e15d5529-bdaf-4d9d-a53f-a8864ec66478" xmlns:ns3="d3fc4b62-afde-4d0a-b311-d84c0759faf2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="20035b3b5f1dea572bd5bfdac2fbef1b" ns2:_="" ns3:_="">
     <xsd:import namespace="e15d5529-bdaf-4d9d-a53f-a8864ec66478"/>
@@ -14392,6 +14383,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A122C20D-CA65-438C-8987-CA60D6F5CFCB}">
   <ds:schemaRefs>
@@ -14402,14 +14402,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F67551D-9961-4E6F-8787-417C33DFD7BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E3D272-C267-4A9B-B8D3-2A1FB2B40D1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14426,4 +14418,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F67551D-9961-4E6F-8787-417C33DFD7BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
new charts for all scenarios
</commit_message>
<xml_diff>
--- a/analysis/library/pipeline/wc-pipeline.xlsx
+++ b/analysis/library/pipeline/wc-pipeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\West Coast ports\Analysis\Deployment\CORAL\analysis\library\pipeline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhemez/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855A8DA3-5BA6-431B-AD2F-9BA0D523947C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36ECA0FE-EFDC-7A40-90F1-AF743403BCFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="6" xr2:uid="{43706732-BCAE-BD4D-8F24-E09A39FF26FB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25580" windowHeight="17300" firstSheet="3" activeTab="6" xr2:uid="{43706732-BCAE-BD4D-8F24-E09A39FF26FB}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="4" r:id="rId1"/>
@@ -786,7 +786,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Baseline-limited-ports"/>
@@ -1160,7 +1160,7 @@
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -1174,7 +1174,7 @@
     <col min="16" max="16" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1374,49 +1374,49 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="M16" s="20"/>
     </row>
-    <row r="43" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="43" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P43" s="12"/>
     </row>
-    <row r="44" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="44" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P44" s="12"/>
     </row>
-    <row r="45" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="45" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P45" s="12"/>
     </row>
-    <row r="46" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="46" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P46" s="12"/>
     </row>
-    <row r="47" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="47" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P47" s="12"/>
     </row>
-    <row r="48" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="48" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P48" s="12"/>
     </row>
-    <row r="49" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="49" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P49" s="12"/>
     </row>
-    <row r="50" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="50" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P50" s="12"/>
     </row>
-    <row r="51" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="51" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P51" s="12"/>
     </row>
-    <row r="52" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="52" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P52" s="12"/>
     </row>
-    <row r="53" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="53" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P53" s="12"/>
     </row>
-    <row r="54" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="54" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P54" s="12"/>
     </row>
-    <row r="55" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="55" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P55" s="12"/>
     </row>
-    <row r="56" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="56" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P56" s="12"/>
     </row>
   </sheetData>
@@ -1432,7 +1432,7 @@
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -1448,7 +1448,7 @@
     <col min="18" max="18" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -2929,46 +2929,46 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="33" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R33" s="12"/>
     </row>
-    <row r="34" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="34" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R34" s="12"/>
     </row>
-    <row r="35" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="35" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R35" s="12"/>
     </row>
-    <row r="36" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="36" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R36" s="12"/>
     </row>
-    <row r="37" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="37" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R37" s="12"/>
     </row>
-    <row r="38" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="38" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R38" s="12"/>
     </row>
-    <row r="39" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="39" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R39" s="12"/>
     </row>
-    <row r="40" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="40" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R40" s="12"/>
     </row>
-    <row r="41" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="41" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R41" s="12"/>
     </row>
-    <row r="42" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="42" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R42" s="12"/>
     </row>
-    <row r="43" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="43" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R43" s="12"/>
     </row>
-    <row r="44" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="44" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R44" s="12"/>
     </row>
-    <row r="45" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="45" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R45" s="12"/>
     </row>
-    <row r="46" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="46" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R46" s="12"/>
     </row>
   </sheetData>
@@ -2984,7 +2984,7 @@
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -3000,7 +3000,7 @@
     <col min="18" max="18" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -3686,7 +3686,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -3857,7 +3857,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -4142,7 +4142,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -4258,7 +4258,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -4316,7 +4316,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -4374,7 +4374,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -4432,7 +4432,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -4490,46 +4490,46 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="33" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R33" s="12"/>
     </row>
-    <row r="34" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="34" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R34" s="12"/>
     </row>
-    <row r="35" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="35" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R35" s="12"/>
     </row>
-    <row r="36" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="36" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R36" s="12"/>
     </row>
-    <row r="37" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="37" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R37" s="12"/>
     </row>
-    <row r="38" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="38" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R38" s="12"/>
     </row>
-    <row r="39" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="39" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R39" s="12"/>
     </row>
-    <row r="40" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="40" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R40" s="12"/>
     </row>
-    <row r="41" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="41" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R41" s="12"/>
     </row>
-    <row r="42" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="42" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R42" s="12"/>
     </row>
-    <row r="43" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="43" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R43" s="12"/>
     </row>
-    <row r="44" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="44" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R44" s="12"/>
     </row>
-    <row r="45" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="45" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R45" s="12"/>
     </row>
-    <row r="46" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="46" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R46" s="12"/>
     </row>
   </sheetData>
@@ -4545,7 +4545,7 @@
       <selection activeCell="P36" sqref="P36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -4561,7 +4561,7 @@
     <col min="18" max="18" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -4617,7 +4617,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -4676,7 +4676,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -4851,7 +4851,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -4908,7 +4908,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -4965,7 +4965,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -5022,7 +5022,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -5136,7 +5136,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -5250,7 +5250,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -5307,7 +5307,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -5364,7 +5364,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -5421,7 +5421,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -5535,7 +5535,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -5592,7 +5592,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -5649,7 +5649,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -5706,7 +5706,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -5824,7 +5824,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -5883,7 +5883,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -5942,7 +5942,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -6001,7 +6001,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -6060,46 +6060,46 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="33" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R33" s="12"/>
     </row>
-    <row r="34" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="34" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R34" s="12"/>
     </row>
-    <row r="35" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="35" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R35" s="12"/>
     </row>
-    <row r="36" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="36" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R36" s="12"/>
     </row>
-    <row r="37" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="37" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R37" s="12"/>
     </row>
-    <row r="38" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="38" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R38" s="12"/>
     </row>
-    <row r="39" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="39" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R39" s="12"/>
     </row>
-    <row r="40" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="40" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R40" s="12"/>
     </row>
-    <row r="41" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="41" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R41" s="12"/>
     </row>
-    <row r="42" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="42" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R42" s="12"/>
     </row>
-    <row r="43" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="43" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R43" s="12"/>
     </row>
-    <row r="44" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="44" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R44" s="12"/>
     </row>
-    <row r="45" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="45" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R45" s="12"/>
     </row>
-    <row r="46" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="46" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R46" s="12"/>
     </row>
   </sheetData>
@@ -6116,7 +6116,7 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -6132,7 +6132,7 @@
     <col min="18" max="18" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -6188,7 +6188,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -6247,7 +6247,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -6365,7 +6365,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -6422,7 +6422,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -6479,7 +6479,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -6536,7 +6536,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -6593,7 +6593,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -6650,7 +6650,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -6707,7 +6707,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -6764,7 +6764,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -6821,7 +6821,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -6878,7 +6878,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -6935,7 +6935,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -6992,7 +6992,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -7049,7 +7049,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -7106,7 +7106,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -7163,7 +7163,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -7220,7 +7220,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -7277,7 +7277,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -7334,7 +7334,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -7391,7 +7391,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -7448,7 +7448,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -7505,7 +7505,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -7562,7 +7562,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -7619,7 +7619,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -7676,7 +7676,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -7733,7 +7733,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -7790,7 +7790,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -7847,7 +7847,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -7906,7 +7906,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -7965,7 +7965,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -8024,7 +8024,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -8083,7 +8083,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -8142,7 +8142,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>53</v>
       </c>
@@ -8201,77 +8201,77 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C37" s="22"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C38" s="22"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C39" s="22"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C40" s="22"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C41" s="22"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C42" s="22"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C43" s="22"/>
       <c r="R43" s="12"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C44" s="22"/>
       <c r="R44" s="12"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C45" s="22"/>
       <c r="R45" s="12"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C46" s="22"/>
       <c r="R46" s="12"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C47" s="22"/>
       <c r="R47" s="12"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C48" s="22"/>
       <c r="R48" s="12"/>
     </row>
-    <row r="49" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C49" s="22"/>
       <c r="R49" s="12"/>
     </row>
-    <row r="50" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C50" s="22"/>
       <c r="R50" s="12"/>
     </row>
-    <row r="51" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C51" s="22"/>
       <c r="R51" s="12"/>
     </row>
-    <row r="52" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C52" s="22"/>
       <c r="R52" s="12"/>
     </row>
-    <row r="53" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C53" s="22"/>
       <c r="R53" s="12"/>
     </row>
-    <row r="54" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C54" s="22"/>
       <c r="R54" s="12"/>
     </row>
-    <row r="55" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C55" s="22"/>
       <c r="R55" s="12"/>
     </row>
-    <row r="56" spans="3:18" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C56" s="22"/>
       <c r="R56" s="12"/>
     </row>
@@ -8288,7 +8288,7 @@
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -8304,7 +8304,7 @@
     <col min="18" max="18" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -8360,7 +8360,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -8417,7 +8417,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -8474,7 +8474,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -8531,7 +8531,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -8588,7 +8588,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -8645,7 +8645,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -8702,7 +8702,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -8759,7 +8759,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -8816,7 +8816,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -8873,7 +8873,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -8930,7 +8930,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -8987,7 +8987,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -9044,7 +9044,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -9101,7 +9101,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -9158,7 +9158,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -9215,7 +9215,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -9272,7 +9272,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -9329,7 +9329,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -9386,7 +9386,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -9443,7 +9443,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -9500,7 +9500,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -9557,7 +9557,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -9614,7 +9614,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -9671,7 +9671,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -9728,7 +9728,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -9785,7 +9785,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -9842,7 +9842,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -9899,7 +9899,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -9956,7 +9956,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -10013,7 +10013,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -10070,7 +10070,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -10127,7 +10127,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -10184,7 +10184,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -10241,7 +10241,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -10298,7 +10298,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>53</v>
       </c>
@@ -10355,46 +10355,46 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="R43" s="12"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="R44" s="12"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="R45" s="12"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="R46" s="12"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="R47" s="12"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="R48" s="12"/>
     </row>
-    <row r="49" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="49" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R49" s="12"/>
     </row>
-    <row r="50" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="50" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R50" s="12"/>
     </row>
-    <row r="51" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="51" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R51" s="12"/>
     </row>
-    <row r="52" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="52" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R52" s="12"/>
     </row>
-    <row r="53" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="53" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R53" s="12"/>
     </row>
-    <row r="54" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="54" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R54" s="12"/>
     </row>
-    <row r="55" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="55" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R55" s="12"/>
     </row>
-    <row r="56" spans="18:18" x14ac:dyDescent="0.35">
+    <row r="56" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R56" s="12"/>
     </row>
   </sheetData>
@@ -10406,11 +10406,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E82BF5EA-4470-6E42-B4F0-EB0C845CDB6E}">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="O50" sqref="O49:O50"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="92" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -10426,7 +10426,7 @@
     <col min="18" max="18" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -10482,7 +10482,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -10539,7 +10539,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -10596,7 +10596,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -10653,7 +10653,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -10710,7 +10710,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -10767,7 +10767,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -10824,7 +10824,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -10881,7 +10881,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -10938,7 +10938,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -10995,7 +10995,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -11052,7 +11052,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -11109,7 +11109,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -11166,7 +11166,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -11223,7 +11223,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -11280,7 +11280,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -11337,7 +11337,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -11394,7 +11394,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -11451,7 +11451,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -11508,7 +11508,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -11565,7 +11565,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -11622,7 +11622,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -11679,7 +11679,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -11736,7 +11736,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -11793,7 +11793,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -11850,7 +11850,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -11907,7 +11907,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -11964,7 +11964,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -12021,7 +12021,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -12078,7 +12078,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -12135,7 +12135,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -12192,7 +12192,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -12249,7 +12249,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -12306,7 +12306,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -12363,7 +12363,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -12420,7 +12420,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>53</v>
       </c>
@@ -12477,7 +12477,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -12534,7 +12534,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>55</v>
       </c>
@@ -12591,7 +12591,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>56</v>
       </c>
@@ -12648,7 +12648,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>57</v>
       </c>
@@ -12705,7 +12705,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>58</v>
       </c>
@@ -12762,7 +12762,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>59</v>
       </c>
@@ -12819,7 +12819,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>60</v>
       </c>
@@ -12879,7 +12879,7 @@
       </c>
       <c r="R43" s="12"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>61</v>
       </c>
@@ -12939,7 +12939,7 @@
       </c>
       <c r="R44" s="12"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>62</v>
       </c>
@@ -12999,7 +12999,7 @@
       </c>
       <c r="R45" s="12"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>63</v>
       </c>
@@ -13059,7 +13059,7 @@
       </c>
       <c r="R46" s="12"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>64</v>
       </c>
@@ -13119,7 +13119,7 @@
       </c>
       <c r="R47" s="12"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>65</v>
       </c>
@@ -13179,7 +13179,7 @@
       </c>
       <c r="R48" s="12"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>66</v>
       </c>
@@ -13239,7 +13239,7 @@
       </c>
       <c r="R49" s="12"/>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>67</v>
       </c>
@@ -13299,7 +13299,7 @@
       </c>
       <c r="R50" s="12"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>68</v>
       </c>
@@ -13359,7 +13359,7 @@
       </c>
       <c r="R51" s="12"/>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>69</v>
       </c>
@@ -13419,7 +13419,7 @@
       </c>
       <c r="R52" s="12"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>70</v>
       </c>
@@ -13479,7 +13479,7 @@
       </c>
       <c r="R53" s="12"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>71</v>
       </c>
@@ -13539,7 +13539,7 @@
       </c>
       <c r="R54" s="12"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>72</v>
       </c>
@@ -13599,7 +13599,7 @@
       </c>
       <c r="R55" s="12"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>73</v>
       </c>
@@ -13672,7 +13672,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
@@ -13686,12 +13686,12 @@
     <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -13702,7 +13702,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -13710,7 +13710,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>81</v>
       </c>
@@ -13718,7 +13718,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>83</v>
       </c>
@@ -13726,7 +13726,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>100</v>
       </c>
@@ -13753,7 +13753,7 @@
       </c>
       <c r="O8" s="27"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
       <c r="B9" s="6"/>
       <c r="C9" s="4" t="s">
@@ -13796,7 +13796,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="28" t="s">
         <v>101</v>
       </c>
@@ -13823,7 +13823,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="28"/>
       <c r="B11" s="5" t="s">
         <v>97</v>
@@ -13848,7 +13848,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="28"/>
       <c r="B12" s="5" t="s">
         <v>98</v>
@@ -13875,7 +13875,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="28"/>
       <c r="B13" s="5" t="s">
         <v>99</v>
@@ -13904,7 +13904,7 @@
       </c>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="28"/>
       <c r="B14" s="8" t="s">
         <v>14</v>
@@ -13927,10 +13927,10 @@
         <v>109.724</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="1:6" ht="62" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>115</v>
       </c>
@@ -13950,7 +13950,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
         <v>120</v>
       </c>
@@ -13968,7 +13968,7 @@
       </c>
       <c r="F18" s="17"/>
     </row>
-    <row r="19" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>125</v>
       </c>
@@ -13988,7 +13988,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
         <v>131</v>
       </c>
@@ -14008,7 +14008,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
         <v>137</v>
       </c>
@@ -14022,7 +14022,7 @@
         <v>89.117000000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
         <v>138</v>
       </c>
@@ -14042,12 +14042,12 @@
         <v>913</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
         <v>139</v>
       </c>
@@ -14067,7 +14067,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
         <v>151</v>
       </c>
@@ -14077,7 +14077,7 @@
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
         <v>152</v>
       </c>
@@ -14087,7 +14087,7 @@
       <c r="E28" s="24"/>
       <c r="F28" s="13"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
         <v>153</v>
       </c>
@@ -14097,7 +14097,7 @@
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
         <v>154</v>
       </c>
@@ -14107,7 +14107,7 @@
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="13" t="s">
         <v>155</v>
       </c>
@@ -14117,7 +14117,7 @@
       <c r="E31" s="19"/>
       <c r="F31" s="13"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
         <v>156</v>
       </c>
@@ -14127,17 +14127,17 @@
       <c r="E32" s="23"/>
       <c r="F32" s="23"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>142</v>
       </c>
@@ -14151,7 +14151,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -14162,7 +14162,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -14173,7 +14173,7 @@
         <v>2034</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>75</v>
       </c>
@@ -14181,7 +14181,7 @@
         <v>2037</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -14192,7 +14192,7 @@
         <v>2038</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -14213,12 +14213,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F8B0B258EEF50240929BB9F36779FA67" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="12d51bf3efa933eaa519000c321f81ab">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e15d5529-bdaf-4d9d-a53f-a8864ec66478" xmlns:ns3="d3fc4b62-afde-4d0a-b311-d84c0759faf2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="20035b3b5f1dea572bd5bfdac2fbef1b" ns2:_="" ns3:_="">
     <xsd:import namespace="e15d5529-bdaf-4d9d-a53f-a8864ec66478"/>
@@ -14383,6 +14377,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -14393,15 +14393,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A122C20D-CA65-438C-8987-CA60D6F5CFCB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E3D272-C267-4A9B-B8D3-2A1FB2B40D1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14420,6 +14411,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A122C20D-CA65-438C-8987-CA60D6F5CFCB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F67551D-9961-4E6F-8787-417C33DFD7BB}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
modified gantt charts and summary plot
</commit_message>
<xml_diff>
--- a/analysis/library/pipeline/wc-pipeline.xlsx
+++ b/analysis/library/pipeline/wc-pipeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhemez/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhemez/Floating-CORAL/CORAL/analysis/library/pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36ECA0FE-EFDC-7A40-90F1-AF743403BCFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A16BA82-C39B-BC40-A686-A4D8FABFE2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25580" windowHeight="17300" firstSheet="3" activeTab="6" xr2:uid="{43706732-BCAE-BD4D-8F24-E09A39FF26FB}"/>
+    <workbookView xWindow="980" yWindow="500" windowWidth="30900" windowHeight="17840" activeTab="1" xr2:uid="{43706732-BCAE-BD4D-8F24-E09A39FF26FB}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="4" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1623" uniqueCount="160">
   <si>
     <t>lat</t>
   </si>
@@ -531,6 +531,12 @@
   </si>
   <si>
     <t>moderate</t>
+  </si>
+  <si>
+    <t>investment</t>
+  </si>
+  <si>
+    <t>investment_year</t>
   </si>
 </sst>
 </file>
@@ -704,7 +710,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -768,6 +774,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1426,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08AAFB4-9BDF-3A4F-BB35-774A258161B8}">
-  <dimension ref="A1:R46"/>
+  <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="143" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1445,10 +1452,11 @@
     <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.6640625" customWidth="1"/>
+    <col min="19" max="19" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -1501,10 +1509,16 @@
         <v>102</v>
       </c>
       <c r="R1" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="S1" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="T1" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1560,8 +1574,14 @@
       <c r="Q2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R2">
+        <v>1274</v>
+      </c>
+      <c r="S2" s="29">
+        <v>47119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1617,8 +1637,14 @@
       <c r="Q3" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R3">
+        <v>1950</v>
+      </c>
+      <c r="S3" s="29">
+        <v>47484</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1674,8 +1700,14 @@
       <c r="Q4" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R4">
+        <v>1950</v>
+      </c>
+      <c r="S4" s="29">
+        <v>47849</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1731,8 +1763,14 @@
       <c r="Q5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R5">
+        <v>1274</v>
+      </c>
+      <c r="S5" s="29">
+        <v>47119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1788,8 +1826,14 @@
       <c r="Q6" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R6">
+        <v>1950</v>
+      </c>
+      <c r="S6" s="29">
+        <v>47484</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1845,8 +1889,14 @@
       <c r="Q7" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R7">
+        <v>1950</v>
+      </c>
+      <c r="S7" s="29">
+        <v>48214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1902,8 +1952,14 @@
       <c r="Q8" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R8">
+        <v>1950</v>
+      </c>
+      <c r="S8" s="29">
+        <v>48580</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1959,8 +2015,14 @@
       <c r="Q9" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R9">
+        <v>1950</v>
+      </c>
+      <c r="S9" s="29">
+        <v>48945</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -2016,8 +2078,14 @@
       <c r="Q10" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R10">
+        <v>1950</v>
+      </c>
+      <c r="S10" s="29">
+        <v>49310</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2073,8 +2141,14 @@
       <c r="Q11" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R11">
+        <v>1950</v>
+      </c>
+      <c r="S11" s="29">
+        <v>49675</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -2130,8 +2204,14 @@
       <c r="Q12" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R12">
+        <v>1950</v>
+      </c>
+      <c r="S12" s="29">
+        <v>50041</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -2187,8 +2267,14 @@
       <c r="Q13" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R13">
+        <v>1950</v>
+      </c>
+      <c r="S13" s="29">
+        <v>50406</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -2244,8 +2330,14 @@
       <c r="Q14" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R14">
+        <v>1950</v>
+      </c>
+      <c r="S14" s="29">
+        <v>50771</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -2301,8 +2393,14 @@
       <c r="Q15" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R15">
+        <v>1950</v>
+      </c>
+      <c r="S15" s="29">
+        <v>51136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -2358,8 +2456,14 @@
       <c r="Q16" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R16">
+        <v>1950</v>
+      </c>
+      <c r="S16" s="29">
+        <v>51502</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -2415,8 +2519,14 @@
       <c r="Q17" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R17">
+        <v>1950</v>
+      </c>
+      <c r="S17" s="29">
+        <v>51867</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -2472,8 +2582,14 @@
       <c r="Q18" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R18">
+        <v>1950</v>
+      </c>
+      <c r="S18" s="29">
+        <v>52232</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -2529,8 +2645,14 @@
       <c r="Q19" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R19">
+        <v>1950</v>
+      </c>
+      <c r="S19" s="29">
+        <v>52597</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -2586,8 +2708,14 @@
       <c r="Q20" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R20">
+        <v>1950</v>
+      </c>
+      <c r="S20" s="29">
+        <v>52597</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -2643,8 +2771,14 @@
       <c r="Q21" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R21">
+        <v>1950</v>
+      </c>
+      <c r="S21" s="29">
+        <v>48214</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -2700,8 +2834,14 @@
       <c r="Q22" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R22">
+        <v>1950</v>
+      </c>
+      <c r="S22" s="29">
+        <v>414187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -2757,8 +2897,14 @@
       <c r="Q23" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R23">
+        <v>1950</v>
+      </c>
+      <c r="S23" s="29">
+        <v>49675</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -2814,8 +2960,14 @@
       <c r="Q24" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R24">
+        <v>1950</v>
+      </c>
+      <c r="S24" s="29">
+        <v>50406</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -2871,8 +3023,14 @@
       <c r="Q25" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R25">
+        <v>1950</v>
+      </c>
+      <c r="S25" s="29">
+        <v>51136</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -2928,48 +3086,54 @@
       <c r="Q26" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="33" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R33" s="12"/>
-    </row>
-    <row r="34" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R34" s="12"/>
-    </row>
-    <row r="35" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R35" s="12"/>
-    </row>
-    <row r="36" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R36" s="12"/>
-    </row>
-    <row r="37" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R37" s="12"/>
-    </row>
-    <row r="38" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R38" s="12"/>
-    </row>
-    <row r="39" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R39" s="12"/>
-    </row>
-    <row r="40" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R40" s="12"/>
-    </row>
-    <row r="41" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R41" s="12"/>
-    </row>
-    <row r="42" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R42" s="12"/>
-    </row>
-    <row r="43" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R43" s="12"/>
-    </row>
-    <row r="44" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R44" s="12"/>
-    </row>
-    <row r="45" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R45" s="12"/>
-    </row>
-    <row r="46" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R46" s="12"/>
+      <c r="R26">
+        <v>1950</v>
+      </c>
+      <c r="S26" s="29">
+        <v>51867</v>
+      </c>
+    </row>
+    <row r="33" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T33" s="12"/>
+    </row>
+    <row r="34" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T34" s="12"/>
+    </row>
+    <row r="35" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T35" s="12"/>
+    </row>
+    <row r="36" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T36" s="12"/>
+    </row>
+    <row r="37" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T37" s="12"/>
+    </row>
+    <row r="38" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T38" s="12"/>
+    </row>
+    <row r="39" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T39" s="12"/>
+    </row>
+    <row r="40" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T40" s="12"/>
+    </row>
+    <row r="41" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T41" s="12"/>
+    </row>
+    <row r="42" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T42" s="12"/>
+    </row>
+    <row r="43" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T43" s="12"/>
+    </row>
+    <row r="44" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T44" s="12"/>
+    </row>
+    <row r="45" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T45" s="12"/>
+    </row>
+    <row r="46" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T46" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10406,7 +10570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E82BF5EA-4470-6E42-B4F0-EB0C845CDB6E}">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="92" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView zoomScale="92" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
@@ -14213,6 +14377,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F8B0B258EEF50240929BB9F36779FA67" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="12d51bf3efa933eaa519000c321f81ab">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e15d5529-bdaf-4d9d-a53f-a8864ec66478" xmlns:ns3="d3fc4b62-afde-4d0a-b311-d84c0759faf2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="20035b3b5f1dea572bd5bfdac2fbef1b" ns2:_="" ns3:_="">
     <xsd:import namespace="e15d5529-bdaf-4d9d-a53f-a8864ec66478"/>
@@ -14377,22 +14550,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F67551D-9961-4E6F-8787-417C33DFD7BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E3D272-C267-4A9B-B8D3-2A1FB2B40D1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14411,19 +14583,11 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A122C20D-CA65-438C-8987-CA60D6F5CFCB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F67551D-9961-4E6F-8787-417C33DFD7BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert wc-pipeline back to 16 GW in Humboldt
</commit_message>
<xml_diff>
--- a/analysis/library/pipeline/wc-pipeline.xlsx
+++ b/analysis/library/pipeline/wc-pipeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhemez/Floating-CORAL/CORAL/analysis/library/pipeline/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\West Coast ports\Analysis\Deployment\CORAL\analysis\library\pipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C63344-81D5-0B4B-917F-7F17BDF35AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61D6782-346E-4C95-AFAF-600AA28F390C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="500" windowWidth="32620" windowHeight="20500" activeTab="6" xr2:uid="{43706732-BCAE-BD4D-8F24-E09A39FF26FB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{43706732-BCAE-BD4D-8F24-E09A39FF26FB}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="4" r:id="rId1"/>
@@ -622,7 +622,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -650,12 +650,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -735,7 +729,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -790,7 +784,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1192,7 +1185,7 @@
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -1206,7 +1199,7 @@
     <col min="16" max="16" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -1256,7 +1249,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1306,7 +1299,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1356,7 +1349,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1406,49 +1399,49 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="M16" s="20"/>
     </row>
-    <row r="43" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P43" s="12"/>
     </row>
-    <row r="44" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P44" s="12"/>
     </row>
-    <row r="45" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P45" s="12"/>
     </row>
-    <row r="46" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P46" s="12"/>
     </row>
-    <row r="47" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P47" s="12"/>
     </row>
-    <row r="48" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P48" s="12"/>
     </row>
-    <row r="49" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P49" s="12"/>
     </row>
-    <row r="50" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P50" s="12"/>
     </row>
-    <row r="51" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P51" s="12"/>
     </row>
-    <row r="52" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P52" s="12"/>
     </row>
-    <row r="53" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P53" s="12"/>
     </row>
-    <row r="54" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P54" s="12"/>
     </row>
-    <row r="55" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P55" s="12"/>
     </row>
-    <row r="56" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P56" s="12"/>
     </row>
   </sheetData>
@@ -1460,11 +1453,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08AAFB4-9BDF-3A4F-BB35-774A258161B8}">
   <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView topLeftCell="B21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:L26"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -1481,7 +1474,7 @@
     <col min="20" max="20" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -1543,7 +1536,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1606,7 +1599,7 @@
         <v>47119</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1669,7 +1662,7 @@
         <v>47484</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1732,7 +1725,7 @@
         <v>47849</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1795,7 +1788,7 @@
         <v>47119</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1858,7 +1851,7 @@
         <v>47484</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1921,7 +1914,7 @@
         <v>48214</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1984,7 +1977,7 @@
         <v>48580</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2047,7 +2040,7 @@
         <v>48945</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -2110,7 +2103,7 @@
         <v>49310</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2173,7 +2166,7 @@
         <v>49675</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -2236,7 +2229,7 @@
         <v>50041</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -2299,7 +2292,7 @@
         <v>50406</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -2362,7 +2355,7 @@
         <v>50771</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -2425,7 +2418,7 @@
         <v>51136</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -2488,7 +2481,7 @@
         <v>51502</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -2551,7 +2544,7 @@
         <v>51867</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -2614,7 +2607,7 @@
         <v>52232</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -2677,7 +2670,7 @@
         <v>52597</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -2740,7 +2733,7 @@
         <v>52597</v>
       </c>
     </row>
-    <row r="21" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -2803,7 +2796,7 @@
         <v>48214</v>
       </c>
     </row>
-    <row r="22" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -2866,7 +2859,7 @@
         <v>414187</v>
       </c>
     </row>
-    <row r="23" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -2929,7 +2922,7 @@
         <v>49675</v>
       </c>
     </row>
-    <row r="24" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -2992,7 +2985,7 @@
         <v>50406</v>
       </c>
     </row>
-    <row r="25" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -3055,7 +3048,7 @@
         <v>51136</v>
       </c>
     </row>
-    <row r="26" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -3118,46 +3111,46 @@
         <v>51867</v>
       </c>
     </row>
-    <row r="33" spans="20:20" x14ac:dyDescent="0.2">
+    <row r="33" spans="20:20" x14ac:dyDescent="0.35">
       <c r="T33" s="12"/>
     </row>
-    <row r="34" spans="20:20" x14ac:dyDescent="0.2">
+    <row r="34" spans="20:20" x14ac:dyDescent="0.35">
       <c r="T34" s="12"/>
     </row>
-    <row r="35" spans="20:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="20:20" x14ac:dyDescent="0.35">
       <c r="T35" s="12"/>
     </row>
-    <row r="36" spans="20:20" x14ac:dyDescent="0.2">
+    <row r="36" spans="20:20" x14ac:dyDescent="0.35">
       <c r="T36" s="12"/>
     </row>
-    <row r="37" spans="20:20" x14ac:dyDescent="0.2">
+    <row r="37" spans="20:20" x14ac:dyDescent="0.35">
       <c r="T37" s="12"/>
     </row>
-    <row r="38" spans="20:20" x14ac:dyDescent="0.2">
+    <row r="38" spans="20:20" x14ac:dyDescent="0.35">
       <c r="T38" s="12"/>
     </row>
-    <row r="39" spans="20:20" x14ac:dyDescent="0.2">
+    <row r="39" spans="20:20" x14ac:dyDescent="0.35">
       <c r="T39" s="12"/>
     </row>
-    <row r="40" spans="20:20" x14ac:dyDescent="0.2">
+    <row r="40" spans="20:20" x14ac:dyDescent="0.35">
       <c r="T40" s="12"/>
     </row>
-    <row r="41" spans="20:20" x14ac:dyDescent="0.2">
+    <row r="41" spans="20:20" x14ac:dyDescent="0.35">
       <c r="T41" s="12"/>
     </row>
-    <row r="42" spans="20:20" x14ac:dyDescent="0.2">
+    <row r="42" spans="20:20" x14ac:dyDescent="0.35">
       <c r="T42" s="12"/>
     </row>
-    <row r="43" spans="20:20" x14ac:dyDescent="0.2">
+    <row r="43" spans="20:20" x14ac:dyDescent="0.35">
       <c r="T43" s="12"/>
     </row>
-    <row r="44" spans="20:20" x14ac:dyDescent="0.2">
+    <row r="44" spans="20:20" x14ac:dyDescent="0.35">
       <c r="T44" s="12"/>
     </row>
-    <row r="45" spans="20:20" x14ac:dyDescent="0.2">
+    <row r="45" spans="20:20" x14ac:dyDescent="0.35">
       <c r="T45" s="12"/>
     </row>
-    <row r="46" spans="20:20" x14ac:dyDescent="0.2">
+    <row r="46" spans="20:20" x14ac:dyDescent="0.35">
       <c r="T46" s="12"/>
     </row>
   </sheetData>
@@ -3169,11 +3162,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DFFBED1-05E8-4648-AFD7-D5B871AAF55A}">
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:O26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -3189,7 +3182,7 @@
     <col min="18" max="18" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -3245,7 +3238,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -3303,7 +3296,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -3361,7 +3354,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -3419,7 +3412,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -3476,7 +3469,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -3533,7 +3526,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -3590,7 +3583,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -3637,8 +3630,8 @@
         <f>_xlfn.CONCAT([1]Helpers!$B$4,'Baseline-Mid (SC)'!M8)</f>
         <v>05/01/2033</v>
       </c>
-      <c r="O8" s="26" t="s">
-        <v>10</v>
+      <c r="O8" t="s">
+        <v>11</v>
       </c>
       <c r="P8" t="s">
         <v>112</v>
@@ -3650,7 +3643,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -3707,7 +3700,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -3754,8 +3747,8 @@
         <f>_xlfn.CONCAT([1]Helpers!$B$4,'Baseline-Mid (SC)'!M10)</f>
         <v>05/01/2035</v>
       </c>
-      <c r="O10" s="26" t="s">
-        <v>10</v>
+      <c r="O10" t="s">
+        <v>11</v>
       </c>
       <c r="P10" t="s">
         <v>112</v>
@@ -3767,7 +3760,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -3824,7 +3817,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -3881,7 +3874,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -3938,7 +3931,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -3995,7 +3988,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -4052,7 +4045,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -4109,7 +4102,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -4169,7 +4162,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -4216,8 +4209,8 @@
         <f>_xlfn.CONCAT([1]Helpers!$B$4,'Baseline-Mid (SC)'!M18)</f>
         <v>05/01/2043</v>
       </c>
-      <c r="O18" s="26" t="s">
-        <v>10</v>
+      <c r="O18" t="s">
+        <v>11</v>
       </c>
       <c r="P18" t="s">
         <v>112</v>
@@ -4229,7 +4222,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -4289,7 +4282,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -4336,8 +4329,8 @@
         <f>_xlfn.CONCAT([1]Helpers!$B$4,'Baseline-Mid (SC)'!M20)</f>
         <v>05/01/2044</v>
       </c>
-      <c r="O20" s="26" t="s">
-        <v>10</v>
+      <c r="O20" t="s">
+        <v>11</v>
       </c>
       <c r="P20" t="s">
         <v>112</v>
@@ -4349,7 +4342,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="21" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -4408,7 +4401,7 @@
       </c>
       <c r="R21"/>
     </row>
-    <row r="22" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -4467,7 +4460,7 @@
       </c>
       <c r="R22"/>
     </row>
-    <row r="23" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -4526,7 +4519,7 @@
       </c>
       <c r="R23"/>
     </row>
-    <row r="24" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -4585,7 +4578,7 @@
       </c>
       <c r="R24"/>
     </row>
-    <row r="25" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -4644,7 +4637,7 @@
       </c>
       <c r="R25"/>
     </row>
-    <row r="26" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -4703,46 +4696,46 @@
       </c>
       <c r="R26"/>
     </row>
-    <row r="33" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R33" s="12"/>
     </row>
-    <row r="34" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R34" s="12"/>
     </row>
-    <row r="35" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R35" s="12"/>
     </row>
-    <row r="36" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R36" s="12"/>
     </row>
-    <row r="37" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R37" s="12"/>
     </row>
-    <row r="38" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R38" s="12"/>
     </row>
-    <row r="39" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R39" s="12"/>
     </row>
-    <row r="40" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R40" s="12"/>
     </row>
-    <row r="41" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R41" s="12"/>
     </row>
-    <row r="42" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R42" s="12"/>
     </row>
-    <row r="43" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R43" s="12"/>
     </row>
-    <row r="44" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R44" s="12"/>
     </row>
-    <row r="45" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R45" s="12"/>
     </row>
-    <row r="46" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R46" s="12"/>
     </row>
   </sheetData>
@@ -4754,11 +4747,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC05C72-3593-F349-9BDB-7CB43BC7148E}">
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -4774,7 +4767,7 @@
     <col min="18" max="18" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -4830,7 +4823,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -4889,7 +4882,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4948,7 +4941,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -5007,7 +5000,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -5064,7 +5057,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -5121,7 +5114,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -5178,7 +5171,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -5235,7 +5228,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -5292,7 +5285,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -5349,7 +5342,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -5406,7 +5399,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -5463,7 +5456,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -5520,7 +5513,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -5577,7 +5570,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -5634,7 +5627,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -5691,7 +5684,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -5748,7 +5741,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -5805,7 +5798,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -5862,7 +5855,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -5919,7 +5912,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -5978,7 +5971,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -6037,7 +6030,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -6096,7 +6089,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -6155,7 +6148,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -6214,7 +6207,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -6273,46 +6266,46 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R33" s="12"/>
     </row>
-    <row r="34" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R34" s="12"/>
     </row>
-    <row r="35" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R35" s="12"/>
     </row>
-    <row r="36" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R36" s="12"/>
     </row>
-    <row r="37" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R37" s="12"/>
     </row>
-    <row r="38" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R38" s="12"/>
     </row>
-    <row r="39" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R39" s="12"/>
     </row>
-    <row r="40" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R40" s="12"/>
     </row>
-    <row r="41" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R41" s="12"/>
     </row>
-    <row r="42" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R42" s="12"/>
     </row>
-    <row r="43" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R43" s="12"/>
     </row>
-    <row r="44" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R44" s="12"/>
     </row>
-    <row r="45" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R45" s="12"/>
     </row>
-    <row r="46" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R46" s="12"/>
     </row>
   </sheetData>
@@ -6325,11 +6318,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D7E48D-8611-1746-819F-E119B83A8576}">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -6345,7 +6338,7 @@
     <col min="18" max="18" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -6401,7 +6394,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -6460,7 +6453,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -6519,7 +6512,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -6578,7 +6571,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -6635,7 +6628,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -6692,7 +6685,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -6749,7 +6742,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -6806,7 +6799,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -6863,7 +6856,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -6920,7 +6913,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -6977,7 +6970,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -7034,7 +7027,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -7091,7 +7084,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -7148,7 +7141,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -7205,7 +7198,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -7262,7 +7255,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -7319,7 +7312,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -7376,7 +7369,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -7433,7 +7426,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -7490,7 +7483,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -7547,7 +7540,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -7604,7 +7597,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -7661,7 +7654,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -7718,7 +7711,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -7775,7 +7768,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -7832,7 +7825,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -7889,7 +7882,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -7946,7 +7939,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -8003,7 +7996,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -8060,7 +8053,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -8119,7 +8112,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -8178,7 +8171,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -8237,7 +8230,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -8296,7 +8289,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -8355,7 +8348,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>53</v>
       </c>
@@ -8414,77 +8407,77 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C37" s="22"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C38" s="22"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C39" s="22"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C40" s="22"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C41" s="22"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C42" s="22"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C43" s="22"/>
       <c r="R43" s="12"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C44" s="22"/>
       <c r="R44" s="12"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C45" s="22"/>
       <c r="R45" s="12"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C46" s="22"/>
       <c r="R46" s="12"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C47" s="22"/>
       <c r="R47" s="12"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C48" s="22"/>
       <c r="R48" s="12"/>
     </row>
-    <row r="49" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C49" s="22"/>
       <c r="R49" s="12"/>
     </row>
-    <row r="50" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C50" s="22"/>
       <c r="R50" s="12"/>
     </row>
-    <row r="51" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C51" s="22"/>
       <c r="R51" s="12"/>
     </row>
-    <row r="52" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C52" s="22"/>
       <c r="R52" s="12"/>
     </row>
-    <row r="53" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C53" s="22"/>
       <c r="R53" s="12"/>
     </row>
-    <row r="54" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C54" s="22"/>
       <c r="R54" s="12"/>
     </row>
-    <row r="55" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C55" s="22"/>
       <c r="R55" s="12"/>
     </row>
-    <row r="56" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C56" s="22"/>
       <c r="R56" s="12"/>
     </row>
@@ -8497,11 +8490,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99C6903C-897C-8C48-A19D-92BDF8BDB5D7}">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView topLeftCell="J6" zoomScale="133" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -8517,7 +8510,7 @@
     <col min="18" max="18" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -8573,7 +8566,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -8633,7 +8626,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -8690,7 +8683,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -8747,7 +8740,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -8804,7 +8797,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -8861,7 +8854,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -8918,7 +8911,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -8975,7 +8968,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -9032,7 +9025,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -9079,8 +9072,8 @@
         <f>_xlfn.CONCAT([1]Helpers!$B$4,'Moderate-Mid (SC)'!M10)</f>
         <v>05/01/2033</v>
       </c>
-      <c r="O10" s="26" t="s">
-        <v>10</v>
+      <c r="O10" t="s">
+        <v>11</v>
       </c>
       <c r="P10" t="s">
         <v>112</v>
@@ -9089,7 +9082,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -9146,7 +9139,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -9193,8 +9186,8 @@
         <f>_xlfn.CONCAT([1]Helpers!$B$4,'Moderate-Mid (SC)'!M12)</f>
         <v>05/01/2035</v>
       </c>
-      <c r="O12" s="26" t="s">
-        <v>10</v>
+      <c r="O12" t="s">
+        <v>11</v>
       </c>
       <c r="P12" t="s">
         <v>112</v>
@@ -9203,7 +9196,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -9260,7 +9253,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -9307,8 +9300,8 @@
         <f>_xlfn.CONCAT([1]Helpers!$B$4,'Moderate-Mid (SC)'!M14)</f>
         <v>05/01/2037</v>
       </c>
-      <c r="O14" s="26" t="s">
-        <v>10</v>
+      <c r="O14" t="s">
+        <v>11</v>
       </c>
       <c r="P14" t="s">
         <v>112</v>
@@ -9317,7 +9310,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -9374,7 +9367,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -9421,8 +9414,8 @@
         <f>_xlfn.CONCAT([1]Helpers!$B$4,'Moderate-Mid (SC)'!M16)</f>
         <v>05/01/2039</v>
       </c>
-      <c r="O16" s="26" t="s">
-        <v>10</v>
+      <c r="O16" t="s">
+        <v>11</v>
       </c>
       <c r="P16" t="s">
         <v>112</v>
@@ -9431,7 +9424,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -9488,7 +9481,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -9545,7 +9538,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -9602,7 +9595,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -9659,7 +9652,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -9716,7 +9709,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -9773,7 +9766,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -9830,7 +9823,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -9887,7 +9880,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -9944,7 +9937,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -10001,7 +9994,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -10058,7 +10051,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -10115,7 +10108,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -10172,7 +10165,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -10229,7 +10222,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -10286,7 +10279,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -10343,7 +10336,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -10400,7 +10393,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -10457,7 +10450,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -10514,7 +10507,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>53</v>
       </c>
@@ -10571,46 +10564,46 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="R43" s="12"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="R44" s="12"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="R45" s="12"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="R46" s="12"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="R47" s="12"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="R48" s="12"/>
     </row>
-    <row r="49" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="49" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R49" s="12"/>
     </row>
-    <row r="50" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="50" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R50" s="12"/>
     </row>
-    <row r="51" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="51" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R51" s="12"/>
     </row>
-    <row r="52" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="52" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R52" s="12"/>
     </row>
-    <row r="53" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="53" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R53" s="12"/>
     </row>
-    <row r="54" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="54" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R54" s="12"/>
     </row>
-    <row r="55" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="55" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R55" s="12"/>
     </row>
-    <row r="56" spans="18:18" x14ac:dyDescent="0.2">
+    <row r="56" spans="18:18" x14ac:dyDescent="0.35">
       <c r="R56" s="12"/>
     </row>
   </sheetData>
@@ -10622,11 +10615,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E82BF5EA-4470-6E42-B4F0-EB0C845CDB6E}">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="86" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="86" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -10642,7 +10635,7 @@
     <col min="18" max="18" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>109</v>
       </c>
@@ -10698,7 +10691,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -10758,7 +10751,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -10815,7 +10808,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -10872,7 +10865,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -10929,7 +10922,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -10986,7 +10979,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -11043,7 +11036,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -11100,7 +11093,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -11157,7 +11150,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -11204,8 +11197,8 @@
         <f>_xlfn.CONCAT([1]Helpers!$B$4,'Expanded-High'!M10)</f>
         <v>05/01/2033</v>
       </c>
-      <c r="O10" s="26" t="s">
-        <v>10</v>
+      <c r="O10" t="s">
+        <v>11</v>
       </c>
       <c r="P10" t="s">
         <v>112</v>
@@ -11214,7 +11207,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -11261,8 +11254,8 @@
         <f>_xlfn.CONCAT([1]Helpers!$B$4,'Expanded-High'!M11)</f>
         <v>05/01/2034</v>
       </c>
-      <c r="O11" s="26" t="s">
-        <v>15</v>
+      <c r="O11" t="s">
+        <v>11</v>
       </c>
       <c r="P11" t="s">
         <v>112</v>
@@ -11271,7 +11264,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -11318,8 +11311,8 @@
         <f>_xlfn.CONCAT([1]Helpers!$B$4,'Expanded-High'!M12)</f>
         <v>05/01/2035</v>
       </c>
-      <c r="O12" s="26" t="s">
-        <v>10</v>
+      <c r="O12" t="s">
+        <v>11</v>
       </c>
       <c r="P12" t="s">
         <v>112</v>
@@ -11328,7 +11321,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -11385,7 +11378,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -11432,8 +11425,8 @@
         <f>_xlfn.CONCAT([1]Helpers!$B$4,'Expanded-High'!M14)</f>
         <v>05/01/2037</v>
       </c>
-      <c r="O14" s="26" t="s">
-        <v>10</v>
+      <c r="O14" t="s">
+        <v>11</v>
       </c>
       <c r="P14" t="s">
         <v>112</v>
@@ -11442,7 +11435,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -11499,7 +11492,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -11546,8 +11539,8 @@
         <f>_xlfn.CONCAT([1]Helpers!$B$4,'Expanded-High'!M16)</f>
         <v>05/01/2039</v>
       </c>
-      <c r="O16" s="26" t="s">
-        <v>10</v>
+      <c r="O16" t="s">
+        <v>11</v>
       </c>
       <c r="P16" t="s">
         <v>112</v>
@@ -11556,7 +11549,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -11613,7 +11606,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -11661,7 +11654,7 @@
         <v>05/01/2041</v>
       </c>
       <c r="O18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P18" t="s">
         <v>112</v>
@@ -11670,7 +11663,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -11727,7 +11720,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -11784,7 +11777,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -11841,7 +11834,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -11898,7 +11891,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -11955,7 +11948,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -12012,7 +12005,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -12069,7 +12062,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -12126,7 +12119,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -12183,7 +12176,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -12240,7 +12233,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -12297,7 +12290,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -12354,7 +12347,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -12411,7 +12404,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -12468,7 +12461,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -12525,7 +12518,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -12582,7 +12575,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -12639,7 +12632,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>53</v>
       </c>
@@ -12696,7 +12689,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -12753,7 +12746,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>55</v>
       </c>
@@ -12810,7 +12803,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>56</v>
       </c>
@@ -12867,7 +12860,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>57</v>
       </c>
@@ -12924,7 +12917,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>58</v>
       </c>
@@ -12981,7 +12974,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>59</v>
       </c>
@@ -13038,7 +13031,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>60</v>
       </c>
@@ -13098,7 +13091,7 @@
       </c>
       <c r="R43" s="12"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>61</v>
       </c>
@@ -13158,7 +13151,7 @@
       </c>
       <c r="R44" s="12"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>62</v>
       </c>
@@ -13218,7 +13211,7 @@
       </c>
       <c r="R45" s="12"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>63</v>
       </c>
@@ -13278,7 +13271,7 @@
       </c>
       <c r="R46" s="12"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>64</v>
       </c>
@@ -13338,7 +13331,7 @@
       </c>
       <c r="R47" s="12"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>65</v>
       </c>
@@ -13398,7 +13391,7 @@
       </c>
       <c r="R48" s="12"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>66</v>
       </c>
@@ -13458,7 +13451,7 @@
       </c>
       <c r="R49" s="12"/>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>67</v>
       </c>
@@ -13518,7 +13511,7 @@
       </c>
       <c r="R50" s="12"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>68</v>
       </c>
@@ -13578,7 +13571,7 @@
       </c>
       <c r="R51" s="12"/>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>69</v>
       </c>
@@ -13638,7 +13631,7 @@
       </c>
       <c r="R52" s="12"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>70</v>
       </c>
@@ -13698,7 +13691,7 @@
       </c>
       <c r="R53" s="12"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>71</v>
       </c>
@@ -13758,7 +13751,7 @@
       </c>
       <c r="R54" s="12"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>72</v>
       </c>
@@ -13818,7 +13811,7 @@
       </c>
       <c r="R55" s="12"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>73</v>
       </c>
@@ -13892,7 +13885,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
@@ -13906,12 +13899,12 @@
     <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -13922,7 +13915,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -13930,7 +13923,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>81</v>
       </c>
@@ -13938,7 +13931,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>83</v>
       </c>
@@ -13946,34 +13939,34 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>100</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28" t="s">
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28" t="s">
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28" t="s">
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="O8" s="28"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O8" s="27"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="10"/>
       <c r="B9" s="6"/>
       <c r="C9" s="4" t="s">
@@ -14016,8 +14009,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="29" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" s="28" t="s">
         <v>101</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -14043,8 +14036,8 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="29"/>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" s="28"/>
       <c r="B11" s="5" t="s">
         <v>97</v>
       </c>
@@ -14068,8 +14061,8 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="29"/>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="28"/>
       <c r="B12" s="5" t="s">
         <v>98</v>
       </c>
@@ -14095,8 +14088,8 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="29"/>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" s="28"/>
       <c r="B13" s="5" t="s">
         <v>99</v>
       </c>
@@ -14124,8 +14117,8 @@
       </c>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="29"/>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" s="28"/>
       <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
@@ -14147,10 +14140,10 @@
         <v>109.724</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="62" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
         <v>115</v>
       </c>
@@ -14170,7 +14163,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>120</v>
       </c>
@@ -14188,7 +14181,7 @@
       </c>
       <c r="F18" s="17"/>
     </row>
-    <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A19" s="16" t="s">
         <v>125</v>
       </c>
@@ -14208,7 +14201,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A20" s="16" t="s">
         <v>131</v>
       </c>
@@ -14228,7 +14221,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
         <v>137</v>
       </c>
@@ -14242,7 +14235,7 @@
         <v>89.117000000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="s">
         <v>138</v>
       </c>
@@ -14262,12 +14255,12 @@
         <v>913</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
         <v>139</v>
       </c>
@@ -14287,7 +14280,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
         <v>151</v>
       </c>
@@ -14297,7 +14290,7 @@
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
         <v>152</v>
       </c>
@@ -14307,7 +14300,7 @@
       <c r="E28" s="24"/>
       <c r="F28" s="13"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="13" t="s">
         <v>153</v>
       </c>
@@ -14317,7 +14310,7 @@
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
         <v>154</v>
       </c>
@@ -14327,7 +14320,7 @@
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
         <v>155</v>
       </c>
@@ -14337,7 +14330,7 @@
       <c r="E31" s="19"/>
       <c r="F31" s="13"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
         <v>156</v>
       </c>
@@ -14347,17 +14340,17 @@
       <c r="E32" s="23"/>
       <c r="F32" s="23"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>142</v>
       </c>
@@ -14371,7 +14364,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -14382,7 +14375,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -14393,7 +14386,7 @@
         <v>2034</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>75</v>
       </c>
@@ -14401,7 +14394,7 @@
         <v>2037</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -14412,7 +14405,7 @@
         <v>2038</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -14433,12 +14426,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F8B0B258EEF50240929BB9F36779FA67" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="12d51bf3efa933eaa519000c321f81ab">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e15d5529-bdaf-4d9d-a53f-a8864ec66478" xmlns:ns3="d3fc4b62-afde-4d0a-b311-d84c0759faf2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="20035b3b5f1dea572bd5bfdac2fbef1b" ns2:_="" ns3:_="">
     <xsd:import namespace="e15d5529-bdaf-4d9d-a53f-a8864ec66478"/>
@@ -14603,6 +14590,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -14613,15 +14606,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A122C20D-CA65-438C-8987-CA60D6F5CFCB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E3D272-C267-4A9B-B8D3-2A1FB2B40D1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14640,6 +14624,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A122C20D-CA65-438C-8987-CA60D6F5CFCB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F67551D-9961-4E6F-8787-417C33DFD7BB}">
   <ds:schemaRefs>

</xml_diff>